<commit_message>
New updates are done
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mustafacetinkaya/Desktop/"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>FirstName</t>
   </si>
@@ -101,12 +101,64 @@
   </si>
   <si>
     <t>Developer</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>Andy</t>
+  </si>
+  <si>
+    <t>Man</t>
+  </si>
+  <si>
+    <t>Shaun</t>
+  </si>
+  <si>
+    <t>Tressa</t>
+  </si>
+  <si>
+    <t>Latashia</t>
+  </si>
+  <si>
+    <t>Lawerence</t>
+  </si>
+  <si>
+    <t>Karri</t>
+  </si>
+  <si>
+    <t>Huels</t>
+  </si>
+  <si>
+    <t>Destiny</t>
+  </si>
+  <si>
+    <t>Beahan</t>
+  </si>
+  <si>
+    <t>Genaro</t>
+  </si>
+  <si>
+    <t>Schowalter</t>
+  </si>
+  <si>
+    <t>Melvin</t>
+  </si>
+  <si>
+    <t>Hoppe</t>
+  </si>
+  <si>
+    <t>Alan</t>
+  </si>
+  <si>
+    <t>Rempel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -477,7 +529,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE86B2B3-7880-6C40-9771-5732D348279B}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="161" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
@@ -495,16 +547,22 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="D2" t="n">
+        <v>80000.0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -517,6 +575,9 @@
       <c r="C3" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="D3" t="n">
+        <v>160000.0</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -528,6 +589,9 @@
       <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="D4" t="n">
+        <v>240000.0</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -539,6 +603,9 @@
       <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="D5" t="n">
+        <v>320000.0</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -550,6 +617,9 @@
       <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="D6" t="n">
+        <v>400000.0</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -561,6 +631,9 @@
       <c r="C7" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="D7" t="n">
+        <v>480000.0</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -571,6 +644,49 @@
       </c>
       <c r="C8" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="D8" t="n">
+        <v>560000.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>